<commit_message>
finalized links for ActiveBOM
</commit_message>
<xml_diff>
--- a/ECAD/Altium/SoM BaseBoard Prototype V0/Project Outputs for SoM BaseBoard Prototype V0/BOM/Copy of Bill of Materials-SoM BaseBoard Prototype V0.xlsx
+++ b/ECAD/Altium/SoM BaseBoard Prototype V0/Project Outputs for SoM BaseBoard Prototype V0/BOM/Copy of Bill of Materials-SoM BaseBoard Prototype V0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keepi\Downloads\Limbotics\transradial_development\ECAD\Altium\SoM BaseBoard Prototype V0\Project Outputs for SoM BaseBoard Prototype V0\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CAD8B2-676E-4ABE-AF93-A00C7E65DD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63D6B51-B08B-4E9B-9D3B-477DD33C4E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{EA60099D-F54E-4EF5-B3BE-0767AC6458E3}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="24510" windowHeight="15990" xr2:uid="{EA60099D-F54E-4EF5-B3BE-0767AC6458E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-SoM B" sheetId="1" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1318,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>188</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>

</xml_diff>